<commit_message>
Renamed setter, wrote english readme, bit refactor the code
</commit_message>
<xml_diff>
--- a/samples/1_simple/exported_file.xlsx
+++ b/samples/1_simple/exported_file.xlsx
@@ -7,9 +7,9 @@
     <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId4"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId5"/>
-    <sheet name="Лист3" sheetId="3" r:id="rId6"/>
+    <sheet name="Worksheet 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Worksheet 2" sheetId="2" r:id="rId5"/>
+    <sheet name="Worksheet 3" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
@@ -19,7 +19,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1">
   <si>
-    <t>Date: 04-10-2018 - Department: Sales department</t>
+    <t>Date: 05-10-2018 - Department: Sales department</t>
   </si>
 </sst>
 </file>

</xml_diff>